<commit_message>
implementacion de lactura de codigos qr y cambio en procesamiento de ejecucion de subida excel
</commit_message>
<xml_diff>
--- a/Files/Plantillas/Plantilla_Alistamiento.xlsx
+++ b/Files/Plantillas/Plantilla_Alistamiento.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LOGI\Carga Masiva\Masivo Inventario Alistamiento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LogiClientes\Files\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
-    <sheet name="Tablas" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="T_OPERADORES">Tablas!$A$1:$B$8</definedName>
-    <definedName name="T_TIPO_ENVIO">Tablas!$D$1:$E$3</definedName>
+    <definedName name="T_OPERADORES">Hoja2!$A$1:$B$8</definedName>
+    <definedName name="T_TIPO_ENVIO">Hoja2!$D$1:$E$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Guia</t>
   </si>
@@ -162,9 +162,6 @@
     <t>OPERADORES</t>
   </si>
   <si>
-    <t>INTERAPIDISIMO</t>
-  </si>
-  <si>
     <t>TIPO ENVIO</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>CUNDINAMARCA</t>
   </si>
   <si>
-    <t>Accesorios Celular</t>
-  </si>
-  <si>
     <t>MASLOGISTICA</t>
   </si>
   <si>
@@ -228,25 +222,19 @@
     <t>LOGI</t>
   </si>
   <si>
-    <t>FUSG0029</t>
-  </si>
-  <si>
-    <t>EF-ZG985CBEGUS</t>
-  </si>
-  <si>
     <t>MERCADOLIBRE</t>
   </si>
   <si>
-    <t>Daniel Arturo Silva Gomez</t>
-  </si>
-  <si>
-    <t>Andrés Mauricio Mosquera</t>
-  </si>
-  <si>
-    <t>Calle 19 #2A-10</t>
-  </si>
-  <si>
-    <t>Carrera 46 #94-21</t>
+    <t>ACCESORIOS CELULAR</t>
+  </si>
+  <si>
+    <t>INTERRAPIDISIMO</t>
+  </si>
+  <si>
+    <t>XDSG0028</t>
+  </si>
+  <si>
+    <t>XDSG0026</t>
   </si>
 </sst>
 </file>
@@ -380,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,7 +384,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,7 +393,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -427,6 +416,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -477,6 +476,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -487,6 +496,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -517,6 +536,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -537,16 +566,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -557,46 +576,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -607,46 +586,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -662,86 +601,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1045,21 +904,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U12" sqref="U12"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
@@ -1094,10 +949,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
@@ -1106,103 +961,99 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>40231573372</v>
+      <c r="A2" s="8">
+        <v>40396423028</v>
       </c>
       <c r="B2" s="1">
-        <v>4174397268</v>
+        <v>4360428472</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
+      <c r="R2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="U2" s="1">
         <f t="shared" ref="U2" si="0">VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V2" s="1">
         <f t="shared" ref="V2" si="1">VLOOKUP(G2,T_TIPO_ENVIO,2,FALSE)</f>
@@ -1210,66 +1061,61 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>40231390031</v>
+      <c r="A3" s="8">
+        <v>40371593939</v>
       </c>
       <c r="B3" s="1">
-        <v>4174191043</v>
+        <v>4332198530</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
       </c>
+      <c r="T3" s="1"/>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U43" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
-        <v>4</v>
+        <f t="shared" ref="U3:U4" si="2">VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="V3" s="1">
-        <f t="shared" ref="V3:V43" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
+        <f t="shared" ref="V3:V4" si="3">VLOOKUP(G3,T_TIPO_ENVIO,2,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -1279,8 +1125,6 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1290,14 +1134,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="U4" s="1" t="e">
-        <f t="shared" ref="U4:U10" si="4">VLOOKUP(E4,T_OPERADORES,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V4" s="1" t="e">
-        <f t="shared" ref="V4:V10" si="5">VLOOKUP(G4,T_TIPO_ENVIO,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1305,9 +1142,6 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1317,14 +1151,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="U5" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V5" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
+      <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1332,9 +1159,6 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="7"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1344,35 +1168,29 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="U6" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V6" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="7"/>
-      <c r="U7" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V7" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1382,25 +1200,24 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="U8" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V8" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-      <c r="U9" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V9" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1408,9 +1225,6 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1420,14 +1234,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="U10" s="1" t="e">
-        <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V10" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#N/A</v>
-      </c>
+      <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1435,9 +1242,6 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="7"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1447,6 +1251,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1454,9 +1259,6 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="7"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1466,6 +1268,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1473,16 +1276,16 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="7"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1490,16 +1293,16 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="7"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1507,528 +1310,114 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="7"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="7"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="7"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="7"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="7"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="7"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="7"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="7"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="7"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="7"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="7"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="7"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="7"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="7"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="7"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="7"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="7"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="7"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="7"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="7"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="7"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="7"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
+      <c r="T17" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A42:A1048576 A20 A1:A6 A22:A35 A10:A15 A8 A17 A37:A40">
-    <cfRule type="duplicateValues" dxfId="33" priority="49"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="32" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="duplicateValues" dxfId="31" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="30" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="duplicateValues" dxfId="29" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="28" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="26" priority="24"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="83"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44:C1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="86"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="duplicateValues" dxfId="23" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
-    <cfRule type="duplicateValues" dxfId="22" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A6 A8:A15 A17 A19:A35 A37:A1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B6 B8:B15 B17 B19:B35 B37:B1048576">
-    <cfRule type="duplicateValues" dxfId="20" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C43">
-    <cfRule type="duplicateValues" dxfId="19" priority="94"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B6 B20 B22:B35 B10:B15 B42:B43 B8 B17 B37:B40">
-    <cfRule type="duplicateValues" dxfId="18" priority="95"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="14" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="161"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="19" priority="255"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C1048576">
+    <cfRule type="duplicateValues" dxfId="18" priority="265"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="17" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="16" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="15" priority="294"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="14" priority="295"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="13" priority="296"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="12" priority="297"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2 A4:A5 A7:A14 A16:A1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="304"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1 B4:B5 B7:B14 B16:B1048576">
+    <cfRule type="duplicateValues" dxfId="10" priority="307"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2 A4:A5 A7:A14 A16:A1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="310"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1 B4:B5 B7:B14 B16:B1048576">
+    <cfRule type="duplicateValues" dxfId="8" priority="313"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2038,13 +1427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,14 +1440,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2071,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -2085,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -2101,7 +1487,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2109,7 +1495,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2117,7 +1503,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2125,7 +1511,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -2143,13 +1529,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>